<commit_message>
add and remove an employee from a project not related to an evaluation cycle
</commit_message>
<xml_diff>
--- a/employee-evaluation/src/main/resources/templates/evaluation_cycle_export_template.xlsx
+++ b/employee-evaluation/src/main/resources/templates/evaluation_cycle_export_template.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\CODING\code\java\intern\employee-evaluation\src\main\resources\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5DE15283-1A78-45E1-ADC6-D63C07AB4CB2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{90EFF8B0-C871-4385-A76C-9E61F72D8860}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -333,74 +333,81 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="1" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="1" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -684,8 +691,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:X7"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+    <sheetView tabSelected="1" topLeftCell="K1" workbookViewId="0">
+      <selection activeCell="O13" sqref="O13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -701,327 +708,330 @@
     <col min="9" max="9" width="18.140625" customWidth="1"/>
     <col min="13" max="13" width="44" customWidth="1"/>
     <col min="14" max="14" width="50.140625" customWidth="1"/>
-    <col min="15" max="15" width="30.28515625" customWidth="1"/>
-    <col min="16" max="16" width="38" customWidth="1"/>
-    <col min="17" max="17" width="18.28515625" customWidth="1"/>
+    <col min="15" max="15" width="38" customWidth="1"/>
+    <col min="16" max="16" width="18.28515625" customWidth="1"/>
+    <col min="17" max="17" width="14.140625" customWidth="1"/>
+    <col min="18" max="18" width="18.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:24" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:24" s="23" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="20" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="20" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="20" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="2"/>
-      <c r="E1" s="2"/>
-      <c r="F1" s="1" t="s">
+      <c r="D1" s="20" t="s">
+        <v>22</v>
+      </c>
+      <c r="E1" s="20" t="s">
+        <v>23</v>
+      </c>
+      <c r="F1" s="20" t="s">
         <v>3</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="G1" s="20" t="s">
         <v>4</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="H1" s="20" t="s">
         <v>5</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="I1" s="20" t="s">
         <v>6</v>
       </c>
-      <c r="J1" s="3" t="s">
+      <c r="J1" s="17" t="s">
         <v>7</v>
       </c>
-      <c r="K1" s="4"/>
-      <c r="L1" s="4"/>
-      <c r="M1" s="5"/>
-      <c r="N1" s="3" t="s">
+      <c r="K1" s="21"/>
+      <c r="L1" s="21"/>
+      <c r="M1" s="22"/>
+      <c r="N1" s="17" t="s">
         <v>8</v>
       </c>
-      <c r="O1" s="5"/>
-      <c r="P1" s="1" t="s">
+      <c r="O1" s="22"/>
+      <c r="P1" s="20" t="s">
         <v>9</v>
       </c>
-      <c r="Q1" s="1" t="s">
+      <c r="Q1" s="20" t="s">
         <v>10</v>
       </c>
-      <c r="R1" s="1" t="s">
+      <c r="R1" s="20" t="s">
         <v>11</v>
       </c>
-      <c r="S1" s="1" t="s">
+      <c r="S1" s="20" t="s">
         <v>12</v>
       </c>
-      <c r="T1" s="1" t="s">
+      <c r="T1" s="20" t="s">
         <v>13</v>
       </c>
-      <c r="U1" s="1" t="s">
+      <c r="U1" s="20" t="s">
         <v>14</v>
       </c>
-      <c r="V1" s="1" t="s">
+      <c r="V1" s="20" t="s">
         <v>15</v>
       </c>
-      <c r="W1" s="1" t="s">
+      <c r="W1" s="20" t="s">
         <v>16</v>
       </c>
-      <c r="X1" s="1" t="s">
+      <c r="X1" s="20" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:24" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A2" s="6"/>
-      <c r="B2" s="6"/>
-      <c r="C2" s="6"/>
-      <c r="D2" s="7"/>
-      <c r="E2" s="7"/>
-      <c r="F2" s="6"/>
-      <c r="G2" s="6"/>
-      <c r="H2" s="6"/>
-      <c r="I2" s="6"/>
-      <c r="J2" s="3" t="s">
+    <row r="2" spans="1:24" s="23" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="24"/>
+      <c r="B2" s="24"/>
+      <c r="C2" s="24"/>
+      <c r="D2" s="18"/>
+      <c r="E2" s="18"/>
+      <c r="F2" s="24"/>
+      <c r="G2" s="24"/>
+      <c r="H2" s="24"/>
+      <c r="I2" s="24"/>
+      <c r="J2" s="17" t="s">
         <v>18</v>
       </c>
-      <c r="K2" s="4"/>
-      <c r="L2" s="5"/>
-      <c r="M2" s="8" t="s">
+      <c r="K2" s="21"/>
+      <c r="L2" s="22"/>
+      <c r="M2" s="18" t="s">
         <v>19</v>
       </c>
-      <c r="N2" s="8" t="s">
+      <c r="N2" s="18" t="s">
         <v>20</v>
       </c>
-      <c r="O2" s="8" t="s">
+      <c r="O2" s="18" t="s">
         <v>21</v>
       </c>
-      <c r="P2" s="6"/>
-      <c r="Q2" s="6"/>
-      <c r="R2" s="6"/>
-      <c r="S2" s="6"/>
-      <c r="T2" s="6"/>
-      <c r="U2" s="6"/>
-      <c r="V2" s="6"/>
-      <c r="W2" s="6"/>
-      <c r="X2" s="6"/>
+      <c r="P2" s="24"/>
+      <c r="Q2" s="24"/>
+      <c r="R2" s="24"/>
+      <c r="S2" s="24"/>
+      <c r="T2" s="24"/>
+      <c r="U2" s="24"/>
+      <c r="V2" s="24"/>
+      <c r="W2" s="24"/>
+      <c r="X2" s="24"/>
     </row>
-    <row r="3" spans="1:24" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A3" s="6"/>
-      <c r="B3" s="6"/>
-      <c r="C3" s="6"/>
-      <c r="D3" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="E3" s="7" t="s">
-        <v>23</v>
-      </c>
-      <c r="F3" s="6"/>
-      <c r="G3" s="6"/>
-      <c r="H3" s="6"/>
-      <c r="I3" s="6"/>
-      <c r="J3" s="9" t="s">
+    <row r="3" spans="1:24" s="23" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A3" s="24"/>
+      <c r="B3" s="24"/>
+      <c r="C3" s="24"/>
+      <c r="D3" s="18"/>
+      <c r="E3" s="18"/>
+      <c r="F3" s="24"/>
+      <c r="G3" s="24"/>
+      <c r="H3" s="24"/>
+      <c r="I3" s="24"/>
+      <c r="J3" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="K3" s="10" t="s">
+      <c r="K3" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="L3" s="11" t="s">
+      <c r="L3" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="M3" s="12"/>
-      <c r="N3" s="12"/>
-      <c r="O3" s="12"/>
-      <c r="P3" s="12"/>
-      <c r="Q3" s="12"/>
-      <c r="R3" s="12"/>
-      <c r="S3" s="6"/>
-      <c r="T3" s="6"/>
-      <c r="U3" s="6"/>
-      <c r="V3" s="6"/>
-      <c r="W3" s="6"/>
-      <c r="X3" s="6"/>
+      <c r="M3" s="25"/>
+      <c r="N3" s="25"/>
+      <c r="O3" s="25"/>
+      <c r="P3" s="25"/>
+      <c r="Q3" s="25"/>
+      <c r="R3" s="25"/>
+      <c r="S3" s="24"/>
+      <c r="T3" s="24"/>
+      <c r="U3" s="24"/>
+      <c r="V3" s="24"/>
+      <c r="W3" s="24"/>
+      <c r="X3" s="24"/>
     </row>
-    <row r="4" spans="1:24" ht="42" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="12"/>
-      <c r="B4" s="12"/>
-      <c r="C4" s="12"/>
-      <c r="D4" s="13"/>
-      <c r="E4" s="13"/>
-      <c r="F4" s="12"/>
-      <c r="G4" s="12"/>
-      <c r="H4" s="12"/>
-      <c r="I4" s="12"/>
-      <c r="J4" s="14" t="s">
+    <row r="4" spans="1:24" s="23" customFormat="1" ht="123" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="25"/>
+      <c r="B4" s="25"/>
+      <c r="C4" s="25"/>
+      <c r="D4" s="26"/>
+      <c r="E4" s="26"/>
+      <c r="F4" s="25"/>
+      <c r="G4" s="25"/>
+      <c r="H4" s="25"/>
+      <c r="I4" s="25"/>
+      <c r="J4" s="19" t="s">
         <v>27</v>
       </c>
-      <c r="K4" s="4"/>
-      <c r="L4" s="5"/>
-      <c r="M4" s="15" t="s">
+      <c r="K4" s="21"/>
+      <c r="L4" s="22"/>
+      <c r="M4" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="N4" s="15" t="s">
+      <c r="N4" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="O4" s="15" t="s">
+      <c r="O4" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="P4" s="15" t="s">
+      <c r="P4" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="Q4" s="15" t="s">
+      <c r="Q4" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="R4" s="15" t="s">
+      <c r="R4" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="S4" s="12"/>
-      <c r="T4" s="12"/>
-      <c r="U4" s="12"/>
-      <c r="V4" s="12"/>
-      <c r="W4" s="12"/>
-      <c r="X4" s="12"/>
+      <c r="S4" s="25"/>
+      <c r="T4" s="25"/>
+      <c r="U4" s="25"/>
+      <c r="V4" s="25"/>
+      <c r="W4" s="25"/>
+      <c r="X4" s="25"/>
     </row>
     <row r="5" spans="1:24" ht="210" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="16"/>
-      <c r="B5" s="17"/>
-      <c r="C5" s="17"/>
-      <c r="D5" s="17"/>
-      <c r="E5" s="17"/>
-      <c r="F5" s="17"/>
-      <c r="G5" s="18"/>
-      <c r="H5" s="18"/>
-      <c r="I5" s="18" t="s">
+      <c r="A5" s="5"/>
+      <c r="B5" s="6"/>
+      <c r="C5" s="6"/>
+      <c r="D5" s="6"/>
+      <c r="E5" s="6"/>
+      <c r="F5" s="6"/>
+      <c r="G5" s="7"/>
+      <c r="H5" s="7"/>
+      <c r="I5" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="J5" s="19" t="s">
+      <c r="J5" s="13" t="s">
         <v>35</v>
       </c>
-      <c r="K5" s="4"/>
-      <c r="L5" s="5"/>
-      <c r="M5" s="20" t="s">
+      <c r="K5" s="14"/>
+      <c r="L5" s="15"/>
+      <c r="M5" s="8" t="s">
         <v>36</v>
       </c>
-      <c r="N5" s="20" t="s">
+      <c r="N5" s="8" t="s">
         <v>37</v>
       </c>
-      <c r="O5" s="20" t="s">
+      <c r="O5" s="8" t="s">
         <v>38</v>
       </c>
-      <c r="P5" s="20" t="s">
+      <c r="P5" s="8" t="s">
         <v>39</v>
       </c>
-      <c r="Q5" s="20" t="s">
+      <c r="Q5" s="8" t="s">
         <v>40</v>
       </c>
-      <c r="R5" s="20"/>
-      <c r="S5" s="20"/>
-      <c r="T5" s="21"/>
-      <c r="U5" s="17"/>
-      <c r="V5" s="17"/>
-      <c r="W5" s="17"/>
-      <c r="X5" s="17"/>
+      <c r="R5" s="8"/>
+      <c r="S5" s="8"/>
+      <c r="T5" s="9"/>
+      <c r="U5" s="6"/>
+      <c r="V5" s="6"/>
+      <c r="W5" s="6"/>
+      <c r="X5" s="6"/>
     </row>
     <row r="6" spans="1:24" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A6" s="16"/>
-      <c r="B6" s="17"/>
-      <c r="C6" s="17"/>
-      <c r="D6" s="17"/>
-      <c r="E6" s="17"/>
-      <c r="F6" s="17"/>
-      <c r="G6" s="18" t="s">
+      <c r="A6" s="5"/>
+      <c r="B6" s="6"/>
+      <c r="C6" s="6"/>
+      <c r="D6" s="6"/>
+      <c r="E6" s="6"/>
+      <c r="F6" s="6"/>
+      <c r="G6" s="7" t="s">
         <v>41</v>
       </c>
-      <c r="H6" s="18"/>
-      <c r="I6" s="18"/>
-      <c r="J6" s="22">
+      <c r="H6" s="7"/>
+      <c r="I6" s="7"/>
+      <c r="J6" s="16">
         <v>5</v>
       </c>
-      <c r="K6" s="4"/>
-      <c r="L6" s="5"/>
-      <c r="M6" s="23">
+      <c r="K6" s="14"/>
+      <c r="L6" s="15"/>
+      <c r="M6" s="10">
         <v>5</v>
       </c>
-      <c r="N6" s="23">
+      <c r="N6" s="10">
         <v>5</v>
       </c>
-      <c r="O6" s="23">
+      <c r="O6" s="10">
         <v>5</v>
       </c>
-      <c r="P6" s="23">
+      <c r="P6" s="10">
         <v>5</v>
       </c>
-      <c r="Q6" s="18"/>
-      <c r="R6" s="18"/>
-      <c r="S6" s="18"/>
-      <c r="T6" s="17"/>
-      <c r="U6" s="17"/>
-      <c r="V6" s="17"/>
-      <c r="W6" s="17"/>
-      <c r="X6" s="17"/>
+      <c r="Q6" s="7"/>
+      <c r="R6" s="7"/>
+      <c r="S6" s="7"/>
+      <c r="T6" s="6"/>
+      <c r="U6" s="6"/>
+      <c r="V6" s="6"/>
+      <c r="W6" s="6"/>
+      <c r="X6" s="6"/>
     </row>
     <row r="7" spans="1:24" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A7" s="24"/>
-      <c r="B7" s="25"/>
-      <c r="C7" s="25"/>
-      <c r="D7" s="25"/>
-      <c r="E7" s="25"/>
-      <c r="F7" s="25"/>
-      <c r="G7" s="23" t="s">
+      <c r="A7" s="11"/>
+      <c r="B7" s="12"/>
+      <c r="C7" s="12"/>
+      <c r="D7" s="12"/>
+      <c r="E7" s="12"/>
+      <c r="F7" s="12"/>
+      <c r="G7" s="10" t="s">
         <v>42</v>
       </c>
-      <c r="H7" s="23"/>
-      <c r="I7" s="23"/>
-      <c r="J7" s="22">
+      <c r="H7" s="10"/>
+      <c r="I7" s="10"/>
+      <c r="J7" s="16">
         <v>0.6</v>
       </c>
-      <c r="K7" s="4"/>
-      <c r="L7" s="5"/>
-      <c r="M7" s="23">
+      <c r="K7" s="14"/>
+      <c r="L7" s="15"/>
+      <c r="M7" s="10">
         <v>0.2</v>
       </c>
-      <c r="N7" s="23">
+      <c r="N7" s="10">
         <v>0.1</v>
       </c>
-      <c r="O7" s="23">
+      <c r="O7" s="10">
         <v>0.1</v>
       </c>
-      <c r="P7" s="23">
+      <c r="P7" s="10">
         <v>0.05</v>
       </c>
-      <c r="Q7" s="23"/>
-      <c r="R7" s="23"/>
-      <c r="S7" s="23"/>
-      <c r="T7" s="25"/>
-      <c r="U7" s="25"/>
-      <c r="V7" s="25"/>
-      <c r="W7" s="25"/>
-      <c r="X7" s="25"/>
+      <c r="Q7" s="10"/>
+      <c r="R7" s="10"/>
+      <c r="S7" s="10"/>
+      <c r="T7" s="12"/>
+      <c r="U7" s="12"/>
+      <c r="V7" s="12"/>
+      <c r="W7" s="12"/>
+      <c r="X7" s="12"/>
     </row>
   </sheetData>
-  <mergeCells count="26">
+  <mergeCells count="28">
+    <mergeCell ref="H1:H4"/>
+    <mergeCell ref="N1:O1"/>
+    <mergeCell ref="R1:R3"/>
+    <mergeCell ref="X1:X4"/>
+    <mergeCell ref="O2:O3"/>
+    <mergeCell ref="A1:A4"/>
+    <mergeCell ref="B1:B4"/>
+    <mergeCell ref="C1:C4"/>
+    <mergeCell ref="F1:F4"/>
+    <mergeCell ref="G1:G4"/>
+    <mergeCell ref="D1:D4"/>
+    <mergeCell ref="E1:E4"/>
+    <mergeCell ref="T1:T4"/>
+    <mergeCell ref="U1:U4"/>
+    <mergeCell ref="V1:V4"/>
+    <mergeCell ref="W1:W4"/>
+    <mergeCell ref="I1:I4"/>
+    <mergeCell ref="J1:M1"/>
+    <mergeCell ref="P1:P3"/>
+    <mergeCell ref="Q1:Q3"/>
+    <mergeCell ref="N2:N3"/>
+    <mergeCell ref="J4:L4"/>
+    <mergeCell ref="S1:S4"/>
     <mergeCell ref="J5:L5"/>
     <mergeCell ref="J6:L6"/>
     <mergeCell ref="J7:L7"/>
     <mergeCell ref="J2:L2"/>
     <mergeCell ref="M2:M3"/>
-    <mergeCell ref="N2:N3"/>
-    <mergeCell ref="O2:O3"/>
-    <mergeCell ref="J4:L4"/>
-    <mergeCell ref="S1:S4"/>
-    <mergeCell ref="T1:T4"/>
-    <mergeCell ref="U1:U4"/>
-    <mergeCell ref="V1:V4"/>
-    <mergeCell ref="W1:W4"/>
-    <mergeCell ref="X1:X4"/>
-    <mergeCell ref="I1:I4"/>
-    <mergeCell ref="J1:M1"/>
-    <mergeCell ref="N1:O1"/>
-    <mergeCell ref="P1:P3"/>
-    <mergeCell ref="Q1:Q3"/>
-    <mergeCell ref="R1:R3"/>
-    <mergeCell ref="A1:A4"/>
-    <mergeCell ref="B1:B4"/>
-    <mergeCell ref="C1:C4"/>
-    <mergeCell ref="F1:F4"/>
-    <mergeCell ref="G1:G4"/>
-    <mergeCell ref="H1:H4"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
simple export feature (not styling)
</commit_message>
<xml_diff>
--- a/employee-evaluation/src/main/resources/templates/evaluation_cycle_export_template.xlsx
+++ b/employee-evaluation/src/main/resources/templates/evaluation_cycle_export_template.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\CODING\code\java\intern\employee-evaluation\src\main\resources\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{90EFF8B0-C871-4385-A76C-9E61F72D8860}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{57649C40-E718-40EA-BCF0-2038F3C01C43}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -371,6 +371,36 @@
     <xf numFmtId="0" fontId="4" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -378,36 +408,6 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -691,8 +691,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:X7"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="K1" workbookViewId="0">
-      <selection activeCell="O13" sqref="O13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -714,32 +714,32 @@
     <col min="18" max="18" width="18.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:24" s="23" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="20" t="s">
+    <row r="1" spans="1:24" s="13" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="14" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="20" t="s">
+      <c r="B1" s="14" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="20" t="s">
+      <c r="C1" s="14" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="20" t="s">
+      <c r="D1" s="14" t="s">
         <v>22</v>
       </c>
-      <c r="E1" s="20" t="s">
+      <c r="E1" s="14" t="s">
         <v>23</v>
       </c>
-      <c r="F1" s="20" t="s">
+      <c r="F1" s="14" t="s">
         <v>3</v>
       </c>
-      <c r="G1" s="20" t="s">
+      <c r="G1" s="14" t="s">
         <v>4</v>
       </c>
-      <c r="H1" s="20" t="s">
+      <c r="H1" s="14" t="s">
         <v>5</v>
       </c>
-      <c r="I1" s="20" t="s">
+      <c r="I1" s="14" t="s">
         <v>6</v>
       </c>
       <c r="J1" s="17" t="s">
@@ -747,83 +747,83 @@
       </c>
       <c r="K1" s="21"/>
       <c r="L1" s="21"/>
-      <c r="M1" s="22"/>
+      <c r="M1" s="18"/>
       <c r="N1" s="17" t="s">
         <v>8</v>
       </c>
-      <c r="O1" s="22"/>
-      <c r="P1" s="20" t="s">
+      <c r="O1" s="18"/>
+      <c r="P1" s="14" t="s">
         <v>9</v>
       </c>
-      <c r="Q1" s="20" t="s">
+      <c r="Q1" s="14" t="s">
         <v>10</v>
       </c>
-      <c r="R1" s="20" t="s">
+      <c r="R1" s="14" t="s">
         <v>11</v>
       </c>
-      <c r="S1" s="20" t="s">
+      <c r="S1" s="14" t="s">
         <v>12</v>
       </c>
-      <c r="T1" s="20" t="s">
+      <c r="T1" s="14" t="s">
         <v>13</v>
       </c>
-      <c r="U1" s="20" t="s">
+      <c r="U1" s="14" t="s">
         <v>14</v>
       </c>
-      <c r="V1" s="20" t="s">
+      <c r="V1" s="14" t="s">
         <v>15</v>
       </c>
-      <c r="W1" s="20" t="s">
+      <c r="W1" s="14" t="s">
         <v>16</v>
       </c>
-      <c r="X1" s="20" t="s">
+      <c r="X1" s="14" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:24" s="23" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="24"/>
-      <c r="B2" s="24"/>
-      <c r="C2" s="24"/>
-      <c r="D2" s="18"/>
-      <c r="E2" s="18"/>
-      <c r="F2" s="24"/>
-      <c r="G2" s="24"/>
-      <c r="H2" s="24"/>
-      <c r="I2" s="24"/>
+    <row r="2" spans="1:24" s="13" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="15"/>
+      <c r="B2" s="15"/>
+      <c r="C2" s="15"/>
+      <c r="D2" s="19"/>
+      <c r="E2" s="19"/>
+      <c r="F2" s="15"/>
+      <c r="G2" s="15"/>
+      <c r="H2" s="15"/>
+      <c r="I2" s="15"/>
       <c r="J2" s="17" t="s">
         <v>18</v>
       </c>
       <c r="K2" s="21"/>
-      <c r="L2" s="22"/>
-      <c r="M2" s="18" t="s">
+      <c r="L2" s="18"/>
+      <c r="M2" s="19" t="s">
         <v>19</v>
       </c>
-      <c r="N2" s="18" t="s">
+      <c r="N2" s="19" t="s">
         <v>20</v>
       </c>
-      <c r="O2" s="18" t="s">
+      <c r="O2" s="19" t="s">
         <v>21</v>
       </c>
-      <c r="P2" s="24"/>
-      <c r="Q2" s="24"/>
-      <c r="R2" s="24"/>
-      <c r="S2" s="24"/>
-      <c r="T2" s="24"/>
-      <c r="U2" s="24"/>
-      <c r="V2" s="24"/>
-      <c r="W2" s="24"/>
-      <c r="X2" s="24"/>
+      <c r="P2" s="15"/>
+      <c r="Q2" s="15"/>
+      <c r="R2" s="15"/>
+      <c r="S2" s="15"/>
+      <c r="T2" s="15"/>
+      <c r="U2" s="15"/>
+      <c r="V2" s="15"/>
+      <c r="W2" s="15"/>
+      <c r="X2" s="15"/>
     </row>
-    <row r="3" spans="1:24" s="23" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A3" s="24"/>
-      <c r="B3" s="24"/>
-      <c r="C3" s="24"/>
-      <c r="D3" s="18"/>
-      <c r="E3" s="18"/>
-      <c r="F3" s="24"/>
-      <c r="G3" s="24"/>
-      <c r="H3" s="24"/>
-      <c r="I3" s="24"/>
+    <row r="3" spans="1:24" s="13" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A3" s="15"/>
+      <c r="B3" s="15"/>
+      <c r="C3" s="15"/>
+      <c r="D3" s="19"/>
+      <c r="E3" s="19"/>
+      <c r="F3" s="15"/>
+      <c r="G3" s="15"/>
+      <c r="H3" s="15"/>
+      <c r="I3" s="15"/>
       <c r="J3" s="1" t="s">
         <v>24</v>
       </c>
@@ -833,34 +833,34 @@
       <c r="L3" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="M3" s="25"/>
-      <c r="N3" s="25"/>
-      <c r="O3" s="25"/>
-      <c r="P3" s="25"/>
-      <c r="Q3" s="25"/>
-      <c r="R3" s="25"/>
-      <c r="S3" s="24"/>
-      <c r="T3" s="24"/>
-      <c r="U3" s="24"/>
-      <c r="V3" s="24"/>
-      <c r="W3" s="24"/>
-      <c r="X3" s="24"/>
+      <c r="M3" s="16"/>
+      <c r="N3" s="16"/>
+      <c r="O3" s="16"/>
+      <c r="P3" s="16"/>
+      <c r="Q3" s="16"/>
+      <c r="R3" s="16"/>
+      <c r="S3" s="15"/>
+      <c r="T3" s="15"/>
+      <c r="U3" s="15"/>
+      <c r="V3" s="15"/>
+      <c r="W3" s="15"/>
+      <c r="X3" s="15"/>
     </row>
-    <row r="4" spans="1:24" s="23" customFormat="1" ht="123" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="25"/>
-      <c r="B4" s="25"/>
-      <c r="C4" s="25"/>
-      <c r="D4" s="26"/>
-      <c r="E4" s="26"/>
-      <c r="F4" s="25"/>
-      <c r="G4" s="25"/>
-      <c r="H4" s="25"/>
-      <c r="I4" s="25"/>
-      <c r="J4" s="19" t="s">
+    <row r="4" spans="1:24" s="13" customFormat="1" ht="123" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="16"/>
+      <c r="B4" s="16"/>
+      <c r="C4" s="16"/>
+      <c r="D4" s="20"/>
+      <c r="E4" s="20"/>
+      <c r="F4" s="16"/>
+      <c r="G4" s="16"/>
+      <c r="H4" s="16"/>
+      <c r="I4" s="16"/>
+      <c r="J4" s="22" t="s">
         <v>27</v>
       </c>
       <c r="K4" s="21"/>
-      <c r="L4" s="22"/>
+      <c r="L4" s="18"/>
       <c r="M4" s="4" t="s">
         <v>28</v>
       </c>
@@ -879,12 +879,12 @@
       <c r="R4" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="S4" s="25"/>
-      <c r="T4" s="25"/>
-      <c r="U4" s="25"/>
-      <c r="V4" s="25"/>
-      <c r="W4" s="25"/>
-      <c r="X4" s="25"/>
+      <c r="S4" s="16"/>
+      <c r="T4" s="16"/>
+      <c r="U4" s="16"/>
+      <c r="V4" s="16"/>
+      <c r="W4" s="16"/>
+      <c r="X4" s="16"/>
     </row>
     <row r="5" spans="1:24" ht="210" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="5"/>
@@ -898,11 +898,11 @@
       <c r="I5" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="J5" s="13" t="s">
+      <c r="J5" s="23" t="s">
         <v>35</v>
       </c>
-      <c r="K5" s="14"/>
-      <c r="L5" s="15"/>
+      <c r="K5" s="24"/>
+      <c r="L5" s="25"/>
       <c r="M5" s="8" t="s">
         <v>36</v>
       </c>
@@ -938,11 +938,11 @@
       </c>
       <c r="H6" s="7"/>
       <c r="I6" s="7"/>
-      <c r="J6" s="16">
+      <c r="J6" s="26">
         <v>5</v>
       </c>
-      <c r="K6" s="14"/>
-      <c r="L6" s="15"/>
+      <c r="K6" s="24"/>
+      <c r="L6" s="25"/>
       <c r="M6" s="10">
         <v>5</v>
       </c>
@@ -976,11 +976,11 @@
       </c>
       <c r="H7" s="10"/>
       <c r="I7" s="10"/>
-      <c r="J7" s="16">
+      <c r="J7" s="26">
         <v>0.6</v>
       </c>
-      <c r="K7" s="14"/>
-      <c r="L7" s="15"/>
+      <c r="K7" s="24"/>
+      <c r="L7" s="25"/>
       <c r="M7" s="10">
         <v>0.2</v>
       </c>
@@ -1004,11 +1004,11 @@
     </row>
   </sheetData>
   <mergeCells count="28">
-    <mergeCell ref="H1:H4"/>
-    <mergeCell ref="N1:O1"/>
-    <mergeCell ref="R1:R3"/>
-    <mergeCell ref="X1:X4"/>
-    <mergeCell ref="O2:O3"/>
+    <mergeCell ref="J5:L5"/>
+    <mergeCell ref="J6:L6"/>
+    <mergeCell ref="J7:L7"/>
+    <mergeCell ref="J2:L2"/>
+    <mergeCell ref="M2:M3"/>
     <mergeCell ref="A1:A4"/>
     <mergeCell ref="B1:B4"/>
     <mergeCell ref="C1:C4"/>
@@ -1016,6 +1016,11 @@
     <mergeCell ref="G1:G4"/>
     <mergeCell ref="D1:D4"/>
     <mergeCell ref="E1:E4"/>
+    <mergeCell ref="H1:H4"/>
+    <mergeCell ref="N1:O1"/>
+    <mergeCell ref="R1:R3"/>
+    <mergeCell ref="X1:X4"/>
+    <mergeCell ref="O2:O3"/>
     <mergeCell ref="T1:T4"/>
     <mergeCell ref="U1:U4"/>
     <mergeCell ref="V1:V4"/>
@@ -1027,11 +1032,6 @@
     <mergeCell ref="N2:N3"/>
     <mergeCell ref="J4:L4"/>
     <mergeCell ref="S1:S4"/>
-    <mergeCell ref="J5:L5"/>
-    <mergeCell ref="J6:L6"/>
-    <mergeCell ref="J7:L7"/>
-    <mergeCell ref="J2:L2"/>
-    <mergeCell ref="M2:M3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
export feature with styling
</commit_message>
<xml_diff>
--- a/employee-evaluation/src/main/resources/templates/evaluation_cycle_export_template.xlsx
+++ b/employee-evaluation/src/main/resources/templates/evaluation_cycle_export_template.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\CODING\code\java\intern\employee-evaluation\src\main\resources\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{57649C40-E718-40EA-BCF0-2038F3C01C43}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C12075FC-7F31-4E89-A71E-6045BACA5298}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -392,13 +392,13 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -692,26 +692,27 @@
   <dimension ref="A1:X7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+      <selection sqref="A1:A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="15.42578125" customWidth="1"/>
-    <col min="2" max="2" width="19.42578125" customWidth="1"/>
+    <col min="1" max="1" width="8" customWidth="1"/>
+    <col min="2" max="2" width="15.7109375" customWidth="1"/>
     <col min="3" max="3" width="24" customWidth="1"/>
-    <col min="4" max="4" width="20.85546875" customWidth="1"/>
-    <col min="5" max="5" width="21.42578125" customWidth="1"/>
+    <col min="4" max="4" width="30.28515625" customWidth="1"/>
+    <col min="5" max="5" width="27.5703125" customWidth="1"/>
     <col min="6" max="6" width="13.28515625" customWidth="1"/>
     <col min="7" max="7" width="12" customWidth="1"/>
     <col min="8" max="8" width="12.28515625" customWidth="1"/>
-    <col min="9" max="9" width="18.140625" customWidth="1"/>
+    <col min="9" max="9" width="29.85546875" customWidth="1"/>
     <col min="13" max="13" width="44" customWidth="1"/>
     <col min="14" max="14" width="50.140625" customWidth="1"/>
     <col min="15" max="15" width="38" customWidth="1"/>
     <col min="16" max="16" width="18.28515625" customWidth="1"/>
     <col min="17" max="17" width="14.140625" customWidth="1"/>
     <col min="18" max="18" width="18.140625" customWidth="1"/>
+    <col min="20" max="20" width="24.140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:24" s="13" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
@@ -745,8 +746,8 @@
       <c r="J1" s="17" t="s">
         <v>7</v>
       </c>
-      <c r="K1" s="21"/>
-      <c r="L1" s="21"/>
+      <c r="K1" s="20"/>
+      <c r="L1" s="20"/>
       <c r="M1" s="18"/>
       <c r="N1" s="17" t="s">
         <v>8</v>
@@ -793,7 +794,7 @@
       <c r="J2" s="17" t="s">
         <v>18</v>
       </c>
-      <c r="K2" s="21"/>
+      <c r="K2" s="20"/>
       <c r="L2" s="18"/>
       <c r="M2" s="19" t="s">
         <v>19</v>
@@ -850,16 +851,16 @@
       <c r="A4" s="16"/>
       <c r="B4" s="16"/>
       <c r="C4" s="16"/>
-      <c r="D4" s="20"/>
-      <c r="E4" s="20"/>
+      <c r="D4" s="22"/>
+      <c r="E4" s="22"/>
       <c r="F4" s="16"/>
       <c r="G4" s="16"/>
       <c r="H4" s="16"/>
       <c r="I4" s="16"/>
-      <c r="J4" s="22" t="s">
+      <c r="J4" s="21" t="s">
         <v>27</v>
       </c>
-      <c r="K4" s="21"/>
+      <c r="K4" s="20"/>
       <c r="L4" s="18"/>
       <c r="M4" s="4" t="s">
         <v>28</v>

</xml_diff>